<commit_message>
Restarted the project basically as they perfomance was not fixable with the old method. Now instead of looking at generation cell first it is now wall first. This prevents overlapping walls meaning less rendering. Currently walls are properly generated but there still needs to be something to detect the empty space between walls as a cell. Without cells the chosen Randomized Depth-first algorithm won't work.
</commit_message>
<xml_diff>
--- a/DTT Git Deliverables/DTT-Assessment-Hour-Log.xlsx
+++ b/DTT Git Deliverables/DTT-Assessment-Hour-Log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\Unity Projects\DTT Maze\DTT Git Deliverables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4977431-0190-4DEB-97B6-062D3DACE18A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B6AE952-1B4E-49E7-9D6A-62626B67A450}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Subject</t>
   </si>
@@ -82,6 +82,37 @@
     <t>In this hour I set up the project on Git, resolved an old Sourcetree bug 
 and looked into the different algorithms on the wikipedia page  that was mentioned in the assessment PDF. After which I used my findings on the
 randomized depth-first algorithm to make a small Cell script.</t>
+  </si>
+  <si>
+    <t>Spent 2 hours setting up everything for the maze to generate through a 
+collection of cells and a grid for recursively filling the maze in. Only to 
+reach the part where I setup the camera and stop dead in my tracks due
+to abysmal performance.</t>
+  </si>
+  <si>
+    <t>Started grid generation and testing the size of the maze while completely staying in the view of the camera. Found that performance is giant issue.</t>
+  </si>
+  <si>
+    <t>Any maze larger than 100x100 lags out whatever I throw at it, tried using 
+sprite renderers instead of 3d objects to lower the vertice count and 
+by manually batching everything after the built in static batching happens.
+But it seems I have to start over and this time start with compute shaders,
+as a maze of 250x250 cells will otherwise just not render. This was made
+sure by using the profiler which showed me that I had about 300ms cpu
+waiting time due to rendering alone.</t>
+  </si>
+  <si>
+    <t>Full performance check to see if my maze idea is even possible due to having to render the whole maze at any size.</t>
+  </si>
+  <si>
+    <t>Instead of having cells with walls, I decided a different approach. Now
+the walls are generated seperately and this way there's also no more 
+overlapping walls making the amount of triangles lower. These walls
+are currently generated but I still have to find a way to identify the 
+empty space between the walls as a cell to make the algorithm work.</t>
+  </si>
+  <si>
+    <t>Instead of cell first generation I am now trying wall first generation.</t>
   </si>
 </sst>
 </file>
@@ -424,6 +455,9 @@
     <xf numFmtId="49" fontId="11" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="1" fontId="1" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -435,9 +469,6 @@
     </xf>
     <xf numFmtId="1" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1699,7 +1730,7 @@
   <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1713,22 +1744,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="21"/>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
+      <c r="A1" s="22"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
       <c r="E1" s="10"/>
       <c r="F1" s="2"/>
     </row>
     <row r="2" spans="1:6" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="24"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="25"/>
     </row>
     <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A3" s="16" t="s">
@@ -1758,33 +1789,57 @@
       <c r="C4" s="18">
         <v>45427</v>
       </c>
-      <c r="D4" s="25" t="s">
+      <c r="D4" s="21" t="s">
         <v>8</v>
       </c>
       <c r="E4" s="20"/>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="5"/>
-      <c r="B5" s="17"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="15"/>
+    <row r="5" spans="1:6" ht="52.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="17">
+        <v>2</v>
+      </c>
+      <c r="C5" s="18">
+        <v>45428</v>
+      </c>
+      <c r="D5" s="21" t="s">
+        <v>9</v>
+      </c>
       <c r="E5" s="20"/>
       <c r="F5" s="4"/>
     </row>
-    <row r="6" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="19"/>
-      <c r="B6" s="17"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="15"/>
+    <row r="6" spans="1:6" ht="129" x14ac:dyDescent="0.35">
+      <c r="A6" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="17">
+        <v>2</v>
+      </c>
+      <c r="C6" s="18">
+        <v>45428</v>
+      </c>
+      <c r="D6" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="E6" s="20"/>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="5"/>
-      <c r="B7" s="17"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="15"/>
+    <row r="7" spans="1:6" ht="65.25" x14ac:dyDescent="0.35">
+      <c r="A7" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="17">
+        <v>2</v>
+      </c>
+      <c r="C7" s="18">
+        <v>45429</v>
+      </c>
+      <c r="D7" s="21" t="s">
+        <v>13</v>
+      </c>
       <c r="E7" s="20"/>
       <c r="F7" s="4"/>
     </row>
@@ -1970,7 +2025,7 @@
       </c>
       <c r="B30" s="14">
         <f>SUMIF(E4:E28,"&lt;&gt;x",B4:B28)</f>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>

</xml_diff>

<commit_message>
Built a class called CellFinder that only has one purpose, find all the cells in the current grid and store them. Next up I will use the collection of cells to implement the maze algorithm.
</commit_message>
<xml_diff>
--- a/DTT Git Deliverables/DTT-Assessment-Hour-Log.xlsx
+++ b/DTT Git Deliverables/DTT-Assessment-Hour-Log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\Unity Projects\DTT Maze\DTT Git Deliverables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B6AE952-1B4E-49E7-9D6A-62626B67A450}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EA58406-D31B-456A-87B6-F253FC165DE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Subject</t>
   </si>
@@ -113,6 +113,14 @@
   </si>
   <si>
     <t>Instead of cell first generation I am now trying wall first generation.</t>
+  </si>
+  <si>
+    <t>The walls are generated and the cells are succesfully all found through
+a seperate class with a function that attempts to find all the cells by 
+going through them in the same order they are generated.</t>
+  </si>
+  <si>
+    <t>Finding all cells from knowing where the walls are.</t>
   </si>
 </sst>
 </file>
@@ -1729,8 +1737,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1843,11 +1851,19 @@
       <c r="E7" s="20"/>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="5"/>
-      <c r="B8" s="17"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="15"/>
+    <row r="8" spans="1:6" ht="39.75" x14ac:dyDescent="0.35">
+      <c r="A8" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="17">
+        <v>2</v>
+      </c>
+      <c r="C8" s="18">
+        <v>45429</v>
+      </c>
+      <c r="D8" s="21" t="s">
+        <v>15</v>
+      </c>
       <c r="E8" s="20"/>
       <c r="F8" s="4"/>
     </row>
@@ -2025,7 +2041,7 @@
       </c>
       <c r="B30" s="14">
         <f>SUMIF(E4:E28,"&lt;&gt;x",B4:B28)</f>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>

</xml_diff>

<commit_message>
Cells were counted and stored but their data was not actually implemented leaving them useless. Now each correct wall is assigned to each cell in it's correct orientation.
</commit_message>
<xml_diff>
--- a/DTT Git Deliverables/DTT-Assessment-Hour-Log.xlsx
+++ b/DTT Git Deliverables/DTT-Assessment-Hour-Log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\Unity Projects\DTT Maze\DTT Git Deliverables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EA58406-D31B-456A-87B6-F253FC165DE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C11615DB-19F1-42F5-BC66-7BD8F282358B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Subject</t>
   </si>
@@ -121,6 +121,13 @@
   </si>
   <si>
     <t>Finding all cells from knowing where the walls are.</t>
+  </si>
+  <si>
+    <t>Bugfix for cell array</t>
+  </si>
+  <si>
+    <t>The cells were counted but not properly implemented with their actual
+walls. This is now fixed.</t>
   </si>
 </sst>
 </file>
@@ -1738,7 +1745,7 @@
   <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1867,11 +1874,19 @@
       <c r="E8" s="20"/>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="5"/>
-      <c r="B9" s="17"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="15"/>
+    <row r="9" spans="1:6" ht="27" x14ac:dyDescent="0.35">
+      <c r="A9" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="17">
+        <v>1</v>
+      </c>
+      <c r="C9" s="18">
+        <v>45429</v>
+      </c>
+      <c r="D9" s="21" t="s">
+        <v>18</v>
+      </c>
       <c r="E9" s="20"/>
       <c r="F9" s="4"/>
     </row>
@@ -2041,7 +2056,7 @@
       </c>
       <c r="B30" s="14">
         <f>SUMIF(E4:E28,"&lt;&gt;x",B4:B28)</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>

</xml_diff>

<commit_message>
Cells are now stored in a grid which can be used much much easier to check for neighbours. Also started on a recursive coroutine loop for the first algorithm.
</commit_message>
<xml_diff>
--- a/DTT Git Deliverables/DTT-Assessment-Hour-Log.xlsx
+++ b/DTT Git Deliverables/DTT-Assessment-Hour-Log.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\Unity Projects\DTT Maze\DTT Git Deliverables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C11615DB-19F1-42F5-BC66-7BD8F282358B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9FA8A17-082F-453E-A717-DFC4E0928872}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DTT Test Hour Log" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Subject</t>
   </si>
@@ -128,6 +128,15 @@
   <si>
     <t>The cells were counted but not properly implemented with their actual
 walls. This is now fixed.</t>
+  </si>
+  <si>
+    <t>Realized that with the current cell collection checking where neighbours 
+is really annoying. So I started work on a cell grid that is made from the
+collection of cells. This grid will be used to check possible empty 
+neighbours, making the system ready for pretty much every algorithm.</t>
+  </si>
+  <si>
+    <t>Creating a cell grid from collection of cells.</t>
   </si>
 </sst>
 </file>
@@ -1745,7 +1754,7 @@
   <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1890,11 +1899,19 @@
       <c r="E9" s="20"/>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="5"/>
-      <c r="B10" s="17"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="15"/>
+    <row r="10" spans="1:6" ht="52.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="17">
+        <v>3</v>
+      </c>
+      <c r="C10" s="18">
+        <v>45434</v>
+      </c>
+      <c r="D10" s="21" t="s">
+        <v>19</v>
+      </c>
       <c r="E10" s="20"/>
       <c r="F10" s="4"/>
     </row>
@@ -2056,7 +2073,7 @@
       </c>
       <c r="B30" s="14">
         <f>SUMIF(E4:E28,"&lt;&gt;x",B4:B28)</f>
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>

</xml_diff>

<commit_message>
Fixed a great many issues with cell finding and grid allocation. No more wrong walls added to wrong cells and now the grid will always be usuable in any type of algorithm. Realized depth first without a stack at this size is impossible, that will be the next and possible final addition of the day.
</commit_message>
<xml_diff>
--- a/DTT Git Deliverables/DTT-Assessment-Hour-Log.xlsx
+++ b/DTT Git Deliverables/DTT-Assessment-Hour-Log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\Unity Projects\DTT Maze\DTT Git Deliverables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9FA8A17-082F-453E-A717-DFC4E0928872}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4C857C8-626F-4306-AE6D-B688D6EA36D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Subject</t>
   </si>
@@ -137,6 +137,15 @@
   </si>
   <si>
     <t>Creating a cell grid from collection of cells.</t>
+  </si>
+  <si>
+    <t>Found many wrong integer casts, and poor calculations in my handling
+of finding all the cells and placing them into a grid for ease of access.
+Spent a good two hours fixing all of these and now the randomized 
+depth-first search algorithm is working smoothly.</t>
+  </si>
+  <si>
+    <t>Fixing cell finding and grid construction</t>
   </si>
 </sst>
 </file>
@@ -1753,8 +1762,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1915,11 +1924,19 @@
       <c r="E10" s="20"/>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="5"/>
-      <c r="B11" s="17"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="15"/>
+    <row r="11" spans="1:6" ht="52.5" x14ac:dyDescent="0.35">
+      <c r="A11" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="17">
+        <v>2</v>
+      </c>
+      <c r="C11" s="18">
+        <v>45434</v>
+      </c>
+      <c r="D11" s="21" t="s">
+        <v>21</v>
+      </c>
       <c r="E11" s="20"/>
       <c r="F11" s="4"/>
     </row>
@@ -2073,7 +2090,7 @@
       </c>
       <c r="B30" s="14">
         <f>SUMIF(E4:E28,"&lt;&gt;x",B4:B28)</f>
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>

</xml_diff>

<commit_message>
Fixed any problems remaining with finding the right walls and cells for each possible cell. Added loads of comments. Implemented the Randomized depth-first search algorithm using a stack instead of recursive. Only needs GUI and then it's bonus time.
</commit_message>
<xml_diff>
--- a/DTT Git Deliverables/DTT-Assessment-Hour-Log.xlsx
+++ b/DTT Git Deliverables/DTT-Assessment-Hour-Log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\Unity Projects\DTT Maze\DTT Git Deliverables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4C857C8-626F-4306-AE6D-B688D6EA36D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57E6D04C-527A-4B3D-B5C6-23D6E43E73E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Subject</t>
   </si>
@@ -146,6 +146,16 @@
   </si>
   <si>
     <t>Fixing cell finding and grid construction</t>
+  </si>
+  <si>
+    <t>Finalized all grid and cell collection and also finalized the randomized 
+depth-first search with a stack implementation instead of recursive. 
+Had issues with properly assigning the southern wall as my original 
+was very poorly done. Added a lot of comments across the project.
+Last step is a simple GUI to set the maze parameters and remake mazes.</t>
+  </si>
+  <si>
+    <t>Implemented algorithm and added comments</t>
   </si>
 </sst>
 </file>
@@ -1762,8 +1772,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1940,11 +1950,19 @@
       <c r="E11" s="20"/>
       <c r="F11" s="4"/>
     </row>
-    <row r="12" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="5"/>
-      <c r="B12" s="17"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="15"/>
+    <row r="12" spans="1:6" ht="65.25" x14ac:dyDescent="0.35">
+      <c r="A12" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="17">
+        <v>3</v>
+      </c>
+      <c r="C12" s="18">
+        <v>45435</v>
+      </c>
+      <c r="D12" s="21" t="s">
+        <v>23</v>
+      </c>
       <c r="E12" s="20"/>
       <c r="F12" s="4"/>
     </row>
@@ -2090,7 +2108,7 @@
       </c>
       <c r="B30" s="14">
         <f>SUMIF(E4:E28,"&lt;&gt;x",B4:B28)</f>
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>

</xml_diff>

<commit_message>
Added UI elements with a button for reloading and generation. Also added 2 sliders to determine the width and height of the maze. Only Bonus objectives left.
</commit_message>
<xml_diff>
--- a/DTT Git Deliverables/DTT-Assessment-Hour-Log.xlsx
+++ b/DTT Git Deliverables/DTT-Assessment-Hour-Log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\Unity Projects\DTT Maze\DTT Git Deliverables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57E6D04C-527A-4B3D-B5C6-23D6E43E73E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40025B47-7A15-4983-AFF4-9CCAF26AC1F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Subject</t>
   </si>
@@ -156,6 +156,15 @@
   </si>
   <si>
     <t>Implemented algorithm and added comments</t>
+  </si>
+  <si>
+    <t>Added UI elements to generate maze</t>
+  </si>
+  <si>
+    <t>Added UI elements to set already determined modifiers now through
+buttons and sliders. These correspond to the same settings that are 
+available in the Editor. Added simple reset option that just reloads the
+scene.</t>
   </si>
 </sst>
 </file>
@@ -1772,8 +1781,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1966,11 +1975,19 @@
       <c r="E12" s="20"/>
       <c r="F12" s="4"/>
     </row>
-    <row r="13" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="5"/>
-      <c r="B13" s="17"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="15"/>
+    <row r="13" spans="1:6" ht="52.5" x14ac:dyDescent="0.35">
+      <c r="A13" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="17">
+        <v>2</v>
+      </c>
+      <c r="C13" s="18">
+        <v>45435</v>
+      </c>
+      <c r="D13" s="21" t="s">
+        <v>26</v>
+      </c>
       <c r="E13" s="20"/>
       <c r="F13" s="4"/>
     </row>
@@ -2108,7 +2125,7 @@
       </c>
       <c r="B30" s="14">
         <f>SUMIF(E4:E28,"&lt;&gt;x",B4:B28)</f>
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>

</xml_diff>

<commit_message>
Read online that Wilsons algorithm is the hardest to get right so I figured I'd challenge myself and implement this as an alternative option. Took a while but after carefully going through the steps I managed to figure it out on my own.
</commit_message>
<xml_diff>
--- a/DTT Git Deliverables/DTT-Assessment-Hour-Log.xlsx
+++ b/DTT Git Deliverables/DTT-Assessment-Hour-Log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\Unity Projects\DTT Maze\DTT Git Deliverables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40025B47-7A15-4983-AFF4-9CCAF26AC1F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E46D9FE-CF9F-4721-90FE-D806F59CE6F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
   <si>
     <t>Subject</t>
   </si>
@@ -165,6 +165,26 @@
 buttons and sliders. These correspond to the same settings that are 
 available in the Editor. Added simple reset option that just reloads the
 scene.</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Added Wilsons algorithm</t>
+  </si>
+  <si>
+    <t>Wanted to really challenge myself so I looked up what  the hardest 
+algorithm to implement was according to others online. They all seemed
+to agree that Wilsons was the hardest to get right so I figured I'll add that
+one. They were not lying as it's quite a tricky one but I managed to 
+implement it nonetheless.</t>
+  </si>
+  <si>
+    <t>Added skybox and gradient</t>
+  </si>
+  <si>
+    <t>Added a skybox shader I tend to re-use a lot for small projects and used
+DoTween to attach a animated gradient to all the wall materials.</t>
   </si>
 </sst>
 </file>
@@ -1781,8 +1801,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1999,20 +2019,40 @@
       <c r="E14" s="20"/>
       <c r="F14" s="4"/>
     </row>
-    <row r="15" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="5"/>
-      <c r="B15" s="17"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="20"/>
+    <row r="15" spans="1:6" ht="90.75" x14ac:dyDescent="0.35">
+      <c r="A15" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="17">
+        <v>5</v>
+      </c>
+      <c r="C15" s="18">
+        <v>45439</v>
+      </c>
+      <c r="D15" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="E15" s="20" t="s">
+        <v>27</v>
+      </c>
       <c r="F15" s="4"/>
     </row>
-    <row r="16" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="5"/>
-      <c r="B16" s="17"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="20"/>
+    <row r="16" spans="1:6" ht="27" x14ac:dyDescent="0.35">
+      <c r="A16" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="17">
+        <v>1</v>
+      </c>
+      <c r="C16" s="18">
+        <v>45439</v>
+      </c>
+      <c r="D16" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="E16" s="20" t="s">
+        <v>27</v>
+      </c>
       <c r="F16" s="4"/>
     </row>
     <row r="17" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
@@ -2125,7 +2165,7 @@
       </c>
       <c r="B30" s="14">
         <f>SUMIF(E4:E28,"&lt;&gt;x",B4:B28)</f>
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>

</xml_diff>